<commit_message>
ajout fichier point Taches projet collaboratif
</commit_message>
<xml_diff>
--- a/resources/point Taches projet collaboratif.xlsx
+++ b/resources/point Taches projet collaboratif.xlsx
@@ -11,12 +11,15 @@
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$H$22</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
   <si>
     <t>Date</t>
   </si>
@@ -33,9 +36,6 @@
     <t>Délai ?</t>
   </si>
   <si>
-    <t>Avancement</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Créer fonction </t>
     </r>
@@ -629,6 +629,36 @@
   </si>
   <si>
     <t xml:space="preserve">07/03/2019 à 15h30 </t>
+  </si>
+  <si>
+    <t>Avancement 1</t>
+  </si>
+  <si>
+    <t>Avancement 2</t>
+  </si>
+  <si>
+    <t>07/03/2019 à 15h30</t>
+  </si>
+  <si>
+    <t>07/03/2019 15h30</t>
+  </si>
+  <si>
+    <t>report - 08/03/2019 - Midi</t>
+  </si>
+  <si>
+    <t>report - 08/03/2019 - Midi - faire JS pour sélectionner membre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">report - 08/03/2019 - Midi </t>
+  </si>
+  <si>
+    <t>Modifier le controleur projet pour modifier un projet</t>
+  </si>
+  <si>
+    <t>Corriger procédure stockée</t>
+  </si>
+  <si>
+    <t>Méthode GET</t>
   </si>
 </sst>
 </file>
@@ -722,12 +752,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -751,15 +781,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -776,18 +797,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -795,13 +809,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -846,53 +854,75 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1188,10 +1218,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1201,432 +1231,502 @@
     <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8">
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="60">
+      <c r="B3" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="60">
-      <c r="B3" s="12">
-        <v>43531</v>
-      </c>
-      <c r="C3" s="13" t="s">
+      <c r="D3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="E3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="G3" s="4"/>
+      <c r="H3" s="5"/>
+    </row>
+    <row r="4" spans="2:8" ht="45">
+      <c r="B4" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="8"/>
-    </row>
-    <row r="4" spans="2:8" ht="45">
-      <c r="B4" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="E4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="5"/>
+    </row>
+    <row r="5" spans="2:8" ht="60">
+      <c r="B5" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="D5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="2:8" ht="60">
-      <c r="B5" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="14" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="5"/>
+    </row>
+    <row r="6" spans="2:8" ht="45">
+      <c r="B6" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="D6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="2:8" ht="45">
-      <c r="B6" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="14" t="s">
+      <c r="G6" s="4"/>
+      <c r="H6" s="5"/>
+    </row>
+    <row r="7" spans="2:8" ht="75">
+      <c r="B7" s="13">
+        <v>43531</v>
+      </c>
+      <c r="C7" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="D7" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="45">
+      <c r="B8" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="2:8" ht="60">
-      <c r="B7" s="18">
-        <v>43531</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="21" t="s">
+      <c r="G8" s="19"/>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="9" spans="2:8" ht="60">
+      <c r="B9" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="45">
-      <c r="B8" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="15" t="s">
+      <c r="G9" s="19"/>
+      <c r="H9" s="5"/>
+    </row>
+    <row r="10" spans="2:8" ht="45">
+      <c r="B10" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" spans="2:8" ht="60">
-      <c r="B9" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="G10" s="19"/>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="2:8" ht="45">
+      <c r="B11" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="75">
+      <c r="B12" s="26">
+        <v>43531</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="2:8" ht="38.25">
+      <c r="B13" s="12">
+        <v>43531</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="19"/>
+      <c r="H13" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="104.25" customHeight="1">
+      <c r="B14" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="31"/>
+      <c r="H14" s="33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="60">
+      <c r="B15" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="24"/>
-    </row>
-    <row r="10" spans="2:8" ht="45">
-      <c r="B10" s="17">
-        <v>43531</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="E10" s="15" t="s">
+      <c r="G15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="75">
+      <c r="B16" s="26">
+        <v>43531</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="5"/>
+    </row>
+    <row r="17" spans="2:8" ht="51">
+      <c r="B17" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="11"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="31"/>
+    </row>
+    <row r="18" spans="2:8" ht="75">
+      <c r="B18" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="24"/>
-    </row>
-    <row r="11" spans="2:8" ht="45">
-      <c r="B11" s="25">
-        <v>43531</v>
-      </c>
-      <c r="C11" s="26" t="s">
-        <v>26</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="G18" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" ht="84.75" customHeight="1">
+      <c r="B19" s="20">
+        <v>43531</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F11" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="26"/>
-    </row>
-    <row r="12" spans="2:8" ht="30">
-      <c r="B12" s="30">
-        <v>43531</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="32" t="s">
+      <c r="G19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="45">
+      <c r="B20" s="20">
+        <v>43531</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E20" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="30">
-      <c r="B13" s="30">
-        <v>43531</v>
-      </c>
-      <c r="C13" s="31" t="s">
+      <c r="F20" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="45">
+      <c r="B21" s="32">
+        <v>43531</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="104.25" customHeight="1">
-      <c r="B14" s="34">
-        <v>43531</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="35" t="s">
+      <c r="E21" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="60">
+      <c r="B22" s="32">
+        <v>43531</v>
+      </c>
+      <c r="C22" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="2:8" ht="30">
-      <c r="B15" s="34">
-        <v>43531</v>
-      </c>
-      <c r="C15" s="19" t="s">
+      <c r="H22" s="40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" ht="45">
+      <c r="B23" s="41">
+        <v>43531</v>
+      </c>
+      <c r="C23" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="30">
-      <c r="B16" s="34">
-        <v>43531</v>
-      </c>
-      <c r="C16" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" ht="60">
-      <c r="B17" s="34">
-        <v>43531</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="G17" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="75">
-      <c r="B18" s="36">
-        <v>43531</v>
-      </c>
-      <c r="C18" s="37" t="s">
+      <c r="F23" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="2:7" ht="84.75" customHeight="1">
-      <c r="B19" s="36">
-        <v>43531</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="2:7" ht="51">
-      <c r="B20" s="12">
-        <v>43531</v>
-      </c>
-      <c r="C20" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F20" s="16"/>
-      <c r="G20" s="24"/>
-    </row>
-    <row r="21" spans="2:7" ht="38.25">
-      <c r="B21" s="38">
-        <v>43531</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="2:7" ht="38.25">
-      <c r="B22" s="38">
-        <v>43531</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="39" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="2:7" ht="51">
-      <c r="B23" s="3">
-        <v>43531</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="2:7" ht="30">
-      <c r="B24" s="3"/>
-      <c r="C24" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="10"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" spans="2:8" ht="45">
+      <c r="B24" s="41">
+        <v>43531</v>
+      </c>
+      <c r="C24" s="42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" spans="2:8" ht="30">
+      <c r="B25" s="41">
+        <v>43531</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B23:B24"/>
-  </mergeCells>
+  <autoFilter ref="B2:H22">
+    <sortState ref="B3:H22">
+      <sortCondition ref="E2:E22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification du fichier" point Taches projet collaboratif.xlsx"
</commit_message>
<xml_diff>
--- a/resources/point Taches projet collaboratif.xlsx
+++ b/resources/point Taches projet collaboratif.xlsx
@@ -12,14 +12,14 @@
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$H$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$B$2:$J$2</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="74">
   <si>
     <t>Date</t>
   </si>
@@ -659,13 +659,43 @@
   </si>
   <si>
     <t>Méthode GET</t>
+  </si>
+  <si>
+    <t>Avancement 3</t>
+  </si>
+  <si>
+    <t>bouton "créeerProjet" fonctionne avec le navigateur Chrome - réglé</t>
+  </si>
+  <si>
+    <t>Corriger la base de données pour incrémenter les clés primaires</t>
+  </si>
+  <si>
+    <t>08/03/2019 à 14h21</t>
+  </si>
+  <si>
+    <t>liste des membres sans équipe - report  08/03/2019 à 16h00</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - report  08/03/2019 à 16h00</t>
+  </si>
+  <si>
+    <t>Avancement 4</t>
+  </si>
+  <si>
+    <t>07/03/2019 à 14h21</t>
+  </si>
+  <si>
+    <t>Mise à jour de production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Afficher-filtrer vue formateur </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,6 +760,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -757,7 +793,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -780,24 +816,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -888,9 +911,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -900,21 +920,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -924,6 +929,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1218,24 +1236,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:H25"/>
+  <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.5703125" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="28.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8">
+    <row r="2" spans="2:10" ht="30">
       <c r="B2" s="6" t="s">
         <v>0</v>
       </c>
@@ -1257,8 +1277,14 @@
       <c r="H2" s="6" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="3" spans="2:8" ht="60">
+      <c r="I2" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" ht="60">
       <c r="B3" s="7">
         <v>43531</v>
       </c>
@@ -1276,8 +1302,10 @@
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="2:8" ht="45">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="2:10" ht="45">
       <c r="B4" s="12">
         <v>43531</v>
       </c>
@@ -1295,8 +1323,10 @@
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="2:8" ht="60">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="2:10" ht="60">
       <c r="B5" s="12">
         <v>43531</v>
       </c>
@@ -1314,8 +1344,10 @@
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="5"/>
-    </row>
-    <row r="6" spans="2:8" ht="45">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:10" ht="45">
       <c r="B6" s="12">
         <v>43531</v>
       </c>
@@ -1333,8 +1365,10 @@
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="5"/>
-    </row>
-    <row r="7" spans="2:8" ht="75">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="2:10" ht="75">
       <c r="B7" s="13">
         <v>43531</v>
       </c>
@@ -1353,11 +1387,13 @@
       <c r="G7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="33" t="s">
+      <c r="H7" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="8" spans="2:8" ht="45">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="2:10" ht="45">
       <c r="B8" s="12">
         <v>43531</v>
       </c>
@@ -1375,8 +1411,10 @@
       </c>
       <c r="G8" s="19"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="2:8" ht="60">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="2:10" ht="60">
       <c r="B9" s="12">
         <v>43531</v>
       </c>
@@ -1394,8 +1432,10 @@
       </c>
       <c r="G9" s="19"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="2:8" ht="45">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="2:10" ht="45">
       <c r="B10" s="12">
         <v>43531</v>
       </c>
@@ -1413,8 +1453,10 @@
       </c>
       <c r="G10" s="19"/>
       <c r="H10" s="5"/>
-    </row>
-    <row r="11" spans="2:8" ht="45">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="2:10" ht="45">
       <c r="B11" s="7">
         <v>43531</v>
       </c>
@@ -1431,11 +1473,13 @@
         <v>27</v>
       </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="33" t="s">
+      <c r="H11" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" ht="75">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="2:10" ht="75">
       <c r="B12" s="26">
         <v>43531</v>
       </c>
@@ -1451,8 +1495,12 @@
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5"/>
-    </row>
-    <row r="13" spans="2:8" ht="38.25">
+      <c r="I12" s="40" t="s">
+        <v>67</v>
+      </c>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="2:10" ht="38.25">
       <c r="B13" s="12">
         <v>43531</v>
       </c>
@@ -1469,11 +1517,13 @@
         <v>53</v>
       </c>
       <c r="G13" s="19"/>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" ht="104.25" customHeight="1">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="2:10" ht="104.25" customHeight="1">
       <c r="B14" s="7">
         <v>43531</v>
       </c>
@@ -1490,243 +1540,311 @@
         <v>53</v>
       </c>
       <c r="G14" s="31"/>
-      <c r="H14" s="33" t="s">
+      <c r="H14" s="32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" ht="60">
-      <c r="B15" s="24">
-        <v>43531</v>
-      </c>
-      <c r="C15" s="14" t="s">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="2:10" ht="45">
+      <c r="B15" s="35">
+        <v>43532</v>
+      </c>
+      <c r="C15" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="2:10" ht="45">
+      <c r="B16" s="35">
+        <v>43533</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="39"/>
+      <c r="E16" s="41" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="2:10" ht="60">
+      <c r="B17" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="16" t="s">
+      <c r="E17" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F17" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G17" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H15" s="33" t="s">
+      <c r="H17" s="32" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" ht="75">
-      <c r="B16" s="26">
-        <v>43531</v>
-      </c>
-      <c r="C16" s="27" t="s">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="2:10" ht="75">
+      <c r="B18" s="26">
+        <v>43531</v>
+      </c>
+      <c r="C18" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="3" t="s">
+      <c r="D18" s="2"/>
+      <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="2:8" ht="51">
-      <c r="B17" s="7">
-        <v>43531</v>
-      </c>
-      <c r="C17" s="28" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="2:10" ht="84.75" customHeight="1">
+      <c r="B19" s="7">
+        <v>43531</v>
+      </c>
+      <c r="C19" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="10" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F17" s="11"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="31"/>
-    </row>
-    <row r="18" spans="2:8" ht="75">
-      <c r="B18" s="24">
-        <v>43531</v>
-      </c>
-      <c r="C18" s="14" t="s">
+      <c r="F19" s="11"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10" ht="75">
+      <c r="B20" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D20" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E20" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F20" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G20" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="H18" s="15" t="s">
+      <c r="H20" s="15" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" ht="84.75" customHeight="1">
-      <c r="B19" s="20">
-        <v>43531</v>
-      </c>
-      <c r="C19" s="21" t="s">
+      <c r="I20" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="5"/>
+    </row>
+    <row r="21" spans="2:10" ht="60">
+      <c r="B21" s="20">
+        <v>43531</v>
+      </c>
+      <c r="C21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D21" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E21" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F21" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G21" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H19" s="15" t="s">
+      <c r="H21" s="15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="2:8" ht="45">
-      <c r="B20" s="20">
-        <v>43531</v>
-      </c>
-      <c r="C20" s="21" t="s">
+      <c r="I21" s="42"/>
+      <c r="J21" s="5"/>
+    </row>
+    <row r="22" spans="2:10" ht="45">
+      <c r="B22" s="20">
+        <v>43531</v>
+      </c>
+      <c r="C22" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D22" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E22" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="17" t="s">
+      <c r="F22" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G22" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="15" t="s">
+      <c r="H22" s="15" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="45">
-      <c r="B21" s="32">
-        <v>43531</v>
-      </c>
-      <c r="C21" s="14" t="s">
+      <c r="I22" s="31"/>
+      <c r="J22" s="5"/>
+    </row>
+    <row r="23" spans="2:10" ht="45">
+      <c r="B23" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E23" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F23" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G23" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="H23" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="22" spans="2:8" ht="60">
-      <c r="B22" s="32">
-        <v>43531</v>
-      </c>
-      <c r="C22" s="36" t="s">
+      <c r="I23" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" s="5"/>
+    </row>
+    <row r="24" spans="2:10" ht="60">
+      <c r="B24" s="24">
+        <v>43531</v>
+      </c>
+      <c r="C24" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D22" s="37" t="s">
+      <c r="D24" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E22" s="38" t="s">
+      <c r="E24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F24" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="39" t="s">
+      <c r="G24" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="H22" s="40" t="s">
+      <c r="H24" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="2:8" ht="45">
-      <c r="B23" s="41">
-        <v>43531</v>
-      </c>
-      <c r="C23" s="42" t="s">
+      <c r="I24" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="2:10" ht="45">
+      <c r="B25" s="35">
+        <v>43531</v>
+      </c>
+      <c r="C25" s="36" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D25" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E25" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-    </row>
-    <row r="24" spans="2:8" ht="45">
-      <c r="B24" s="41">
-        <v>43531</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-    </row>
-    <row r="25" spans="2:8" ht="30">
-      <c r="B25" s="41">
-        <v>43531</v>
-      </c>
-      <c r="C25" s="43" t="s">
-        <v>62</v>
-      </c>
-      <c r="D25" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="34" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="34" t="s">
+      <c r="F25" s="33" t="s">
         <v>52</v>
       </c>
       <c r="G25" s="5"/>
       <c r="H25" s="5"/>
+      <c r="I25" s="40" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="31"/>
+    </row>
+    <row r="26" spans="2:10" ht="30">
+      <c r="B26" s="35">
+        <v>43531</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G26" s="5"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+    </row>
+    <row r="27" spans="2:10" ht="60">
+      <c r="B27" s="35">
+        <v>43532</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="39"/>
+      <c r="E27" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27" s="33" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5"/>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H22">
-    <sortState ref="B3:H22">
-      <sortCondition ref="E2:E22"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="B2:J2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>